<commit_message>
Minor edits to code. Re-enter a cell in Input_Matrix_Hilus that had beed deleted accidentaly.
</commit_message>
<xml_diff>
--- a/Input_Matrix_Hilus.xlsx
+++ b/Input_Matrix_Hilus.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98247833-6C47-48F4-AF79-1934A1700078}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A8B984-3E34-4E2F-AF1F-8F69A0A743BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="251">
   <si>
     <t>Date</t>
   </si>
@@ -980,7 +980,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1419,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CO147"/>
+  <dimension ref="A1:CO148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+      <selection activeCell="A148" sqref="A148:XFD148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39155,7 +39179,7 @@
         <v>0</v>
       </c>
       <c r="CO134" s="1">
-        <f t="shared" ref="CO134:CO147" si="3">SUM(AY134:CN134)</f>
+        <f t="shared" ref="CO134:CO148" si="3">SUM(AY134:CN134)</f>
         <v>1</v>
       </c>
     </row>
@@ -42149,32 +42173,273 @@
         <v>4</v>
       </c>
     </row>
+    <row r="148" spans="1:93" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="B148" s="14">
+        <v>40762</v>
+      </c>
+      <c r="C148" s="15">
+        <v>8</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E148" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="F148" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G148" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H148" s="10">
+        <v>0</v>
+      </c>
+      <c r="I148" s="10">
+        <v>0</v>
+      </c>
+      <c r="J148" s="10">
+        <v>0</v>
+      </c>
+      <c r="K148" s="10">
+        <v>-53</v>
+      </c>
+      <c r="L148" s="10">
+        <v>1214.5999999999999</v>
+      </c>
+      <c r="M148" s="10">
+        <v>58.366900000000001</v>
+      </c>
+      <c r="N148" s="10">
+        <v>48.054400000000001</v>
+      </c>
+      <c r="O148" s="10">
+        <v>952.904</v>
+      </c>
+      <c r="P148" s="10">
+        <v>837.505</v>
+      </c>
+      <c r="Q148" s="10">
+        <v>87.889700000000005</v>
+      </c>
+      <c r="R148" s="11">
+        <v>10</v>
+      </c>
+      <c r="S148" s="11">
+        <v>260.98</v>
+      </c>
+      <c r="T148" s="11">
+        <v>-1.09937</v>
+      </c>
+      <c r="U148" s="11">
+        <v>18.2851</v>
+      </c>
+      <c r="V148" s="12">
+        <v>0</v>
+      </c>
+      <c r="W148" s="12">
+        <v>26.134599999999999</v>
+      </c>
+      <c r="X148" s="12">
+        <v>199.684</v>
+      </c>
+      <c r="Y148" s="12">
+        <v>41.825299999999999</v>
+      </c>
+      <c r="Z148" s="12">
+        <v>1.5831299999999999</v>
+      </c>
+      <c r="AA148" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB148" s="12">
+        <v>0</v>
+      </c>
+      <c r="AC148" s="13">
+        <v>77.667199999999994</v>
+      </c>
+      <c r="AD148" s="13">
+        <v>0.90461400000000003</v>
+      </c>
+      <c r="AE148" s="13">
+        <v>-26.6418</v>
+      </c>
+      <c r="AF148" s="13">
+        <v>0</v>
+      </c>
+      <c r="AG148" s="13">
+        <v>0</v>
+      </c>
+      <c r="AH148" s="13">
+        <v>-26.6418</v>
+      </c>
+      <c r="AI148" s="13">
+        <v>3.46</v>
+      </c>
+      <c r="AJ148" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK148" s="13">
+        <v>0</v>
+      </c>
+      <c r="AL148" s="13">
+        <v>3.46</v>
+      </c>
+      <c r="AM148" s="13">
+        <v>72.998000000000005</v>
+      </c>
+      <c r="AN148" s="13">
+        <v>0.98042700000000005</v>
+      </c>
+      <c r="AO148" s="13">
+        <v>-26.184100000000001</v>
+      </c>
+      <c r="AP148" s="13">
+        <v>0</v>
+      </c>
+      <c r="AQ148" s="13">
+        <v>0</v>
+      </c>
+      <c r="AR148" s="13">
+        <v>-26.184100000000001</v>
+      </c>
+      <c r="AS148" s="13">
+        <v>4.22</v>
+      </c>
+      <c r="AT148" s="13">
+        <v>0</v>
+      </c>
+      <c r="AU148" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV148" s="5">
+        <v>4.22</v>
+      </c>
+      <c r="AW148" s="5">
+        <v>6.011804210786522E-2</v>
+      </c>
+      <c r="AX148" s="13">
+        <f t="shared" ref="AX148" si="4">(AN148-AD148)/AD148</f>
+        <v>8.3807016031147E-2</v>
+      </c>
+      <c r="AY148" s="17">
+        <v>0</v>
+      </c>
+      <c r="AZ148" s="17">
+        <v>1</v>
+      </c>
+      <c r="BA148" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB148" s="17">
+        <v>0</v>
+      </c>
+      <c r="BC148" s="17">
+        <v>0</v>
+      </c>
+      <c r="BD148" s="17">
+        <v>0</v>
+      </c>
+      <c r="BE148" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF148" s="17">
+        <v>0</v>
+      </c>
+      <c r="BG148" s="17">
+        <v>0</v>
+      </c>
+      <c r="BH148" s="17">
+        <v>0</v>
+      </c>
+      <c r="BI148" s="17">
+        <v>1</v>
+      </c>
+      <c r="BJ148" s="22"/>
+      <c r="BK148" s="22"/>
+      <c r="BL148" s="17">
+        <v>0</v>
+      </c>
+      <c r="BM148" s="22"/>
+      <c r="BN148" s="22"/>
+      <c r="BO148" s="22"/>
+      <c r="BP148" s="22"/>
+      <c r="BQ148" s="22"/>
+      <c r="BR148" s="22"/>
+      <c r="BS148" s="22"/>
+      <c r="BT148" s="22"/>
+      <c r="BU148" s="22"/>
+      <c r="BV148" s="22"/>
+      <c r="BW148" s="22"/>
+      <c r="BX148" s="22"/>
+      <c r="BY148" s="22"/>
+      <c r="BZ148" s="22"/>
+      <c r="CA148" s="22"/>
+      <c r="CB148" s="22"/>
+      <c r="CC148" s="22"/>
+      <c r="CD148" s="22"/>
+      <c r="CE148" s="22"/>
+      <c r="CF148" s="22"/>
+      <c r="CG148" s="22"/>
+      <c r="CH148" s="22"/>
+      <c r="CI148" s="22"/>
+      <c r="CJ148" s="22"/>
+      <c r="CK148" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL148" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM148" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN148" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO148" s="16">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="AY58:CN73">
+    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:AV7 AY1:CN133 G1:G147 A1:F118 H9:AV118 AH3:AH147 AL3:AL147 AV2:AV147 AR2:AR147 AW1:AX147">
+    <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AY58:CN73">
     <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:AV7 AY1:CN133 G1:G147 A1:F118 H9:AV118 AH3:AH147 AL3:AL147 AV2:AV147 AR2:AR147 AW1:AX147">
-    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="B59:D59 C60:D71 A58:CO58">
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY58:CN73">
-    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59:D59 C60:D71 A58:CO58">
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY2:CN147">
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G148 AH148 AL148 AR148 AV148:AX148">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY148:CN148">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -69827,30 +70092,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="T58:BJ73">
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8 O119:O148 Q8 Q119:Q148 B1:Q7 T1:BJ133 A1:A118 R1:S148 B9:Q118 W3:W148">
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T58:BJ73">
-    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:BK58">
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:BJ148">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>